<commit_message>
project runs waiting for export
</commit_message>
<xml_diff>
--- a/Calculator.WPF/testfile.xlsx
+++ b/Calculator.WPF/testfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\engr\source\repos\UnitCalculator\Calculator.WPF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8FF660-5723-4D3B-88FA-0B7AA624C42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882720C0-8251-4C0E-A4B2-33D9513B7560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,10 +48,10 @@
     <t>km</t>
   </si>
   <si>
+    <t>in</t>
+  </si>
+  <si>
     <t>ft</t>
-  </si>
-  <si>
-    <t>in</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,10 +415,10 @@
         <v>78954</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>